<commit_message>
SQL обновил функцию get_view_outgoing_cars_of_id_sostav
</commit_message>
<xml_diff>
--- a/Documents/Описание ПО/Функции и ХП.xlsx
+++ b/Documents/Описание ПО/Функции и ХП.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Мои документы\Visual Studio 2019\Project\Work\IDS_RailWay\Documents\Описание ПО\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE1200B-D1AC-42F1-8E38-34518ECF29F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5DE717-49CD-4813-92F9-0DBD7595D349}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="51">
   <si>
     <t>Функция</t>
   </si>
@@ -267,6 +267,36 @@
   </si>
   <si>
     <t>Использует</t>
+  </si>
+  <si>
+    <t>[IDS].[get_view_outgoing_cars_of_id_sostav]</t>
+  </si>
+  <si>
+    <t>int @id_sostav</t>
+  </si>
+  <si>
+    <t>Получить полную информацию по вагонам отправляемого состава</t>
+  </si>
+  <si>
+    <t>api/ids/rwt/outgoing_cars/view/sostav/id/</t>
+  </si>
+  <si>
+    <t>IDS_RWT_OutgoingCarsController</t>
+  </si>
+  <si>
+    <t>ids_wsd.prototype.getViewOutgoingCarsOfIDSostav</t>
+  </si>
+  <si>
+    <t>api</t>
+  </si>
+  <si>
+    <t>Controller</t>
+  </si>
+  <si>
+    <t>js module</t>
+  </si>
+  <si>
+    <t>Форма АРМ (отправить на УЗ), Отчеты по отправке.</t>
   </si>
 </sst>
 </file>
@@ -345,7 +375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -367,6 +397,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1023,23 +1056,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E1A7421-E2FD-4C0A-8478-37F11373238D}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.28515625" customWidth="1"/>
     <col min="2" max="2" width="21.140625" customWidth="1"/>
     <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="91.28515625" customWidth="1"/>
+    <col min="4" max="4" width="53.28515625" customWidth="1"/>
     <col min="5" max="5" width="31.7109375" customWidth="1"/>
     <col min="6" max="6" width="39" customWidth="1"/>
+    <col min="7" max="7" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="48.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1058,8 +1094,17 @@
       <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>29</v>
       </c>
@@ -1069,15 +1114,18 @@
       <c r="C2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="8" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>34</v>
       </c>
@@ -1085,15 +1133,18 @@
       <c r="C3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>37</v>
       </c>
@@ -1103,7 +1154,7 @@
       <c r="C4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="8" t="s">
         <v>38</v>
       </c>
       <c r="E4" s="7" t="s">
@@ -1112,8 +1163,105 @@
       <c r="F4" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>